<commit_message>
Model evaluations with darts
</commit_message>
<xml_diff>
--- a/El_Salvador_Financial_Info.xlsx
+++ b/El_Salvador_Financial_Info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkateeb3/Documents/Fintech_Workspace/Project_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkateeb3/Documents/Fintech_Workspace/Project_3/El-Salvador-Financial-Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266F12F4-1465-CC49-9A87-B1413168288E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95DC4FE-3D05-EA4C-9261-68CE7481E71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{6A573F78-A188-5640-A790-3091458354EC}"/>
   </bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D2F96C-5324-6B49-847F-4383C671B3FF}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:CY42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,7 @@
         <v>5561916</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1995</v>
       </c>
@@ -714,7 +714,7 @@
         <v>5628602</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1996</v>
       </c>
@@ -734,7 +734,7 @@
         <v>5689943</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1997</v>
       </c>
@@ -753,8 +753,9 @@
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY19" s="2"/>
+    </row>
+    <row r="20" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1998</v>
       </c>
@@ -775,8 +776,9 @@
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY20" s="3"/>
+    </row>
+    <row r="21" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1999</v>
       </c>
@@ -797,8 +799,9 @@
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY21" s="3"/>
+    </row>
+    <row r="22" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2000</v>
       </c>
@@ -819,8 +822,9 @@
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY22" s="3"/>
+    </row>
+    <row r="23" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2001</v>
       </c>
@@ -841,8 +845,9 @@
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY23" s="3"/>
+    </row>
+    <row r="24" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2002</v>
       </c>
@@ -863,8 +868,9 @@
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY24" s="3"/>
+    </row>
+    <row r="25" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -885,8 +891,9 @@
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY25" s="3"/>
+    </row>
+    <row r="26" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -907,8 +914,9 @@
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY26" s="3"/>
+    </row>
+    <row r="27" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -929,8 +937,9 @@
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY27" s="3"/>
+    </row>
+    <row r="28" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -951,8 +960,9 @@
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY28" s="3"/>
+    </row>
+    <row r="29" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2007</v>
       </c>
@@ -973,8 +983,9 @@
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY29" s="3"/>
+    </row>
+    <row r="30" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2008</v>
       </c>
@@ -995,8 +1006,9 @@
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY30" s="3"/>
+    </row>
+    <row r="31" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2009</v>
       </c>
@@ -1017,8 +1029,9 @@
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY31" s="3"/>
+    </row>
+    <row r="32" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2010</v>
       </c>
@@ -1039,8 +1052,9 @@
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY32" s="3"/>
+    </row>
+    <row r="33" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -1061,8 +1075,9 @@
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY33" s="3"/>
+    </row>
+    <row r="34" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -1083,8 +1098,9 @@
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY34" s="3"/>
+    </row>
+    <row r="35" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2013</v>
       </c>
@@ -1105,8 +1121,9 @@
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY35" s="3"/>
+    </row>
+    <row r="36" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -1127,8 +1144,9 @@
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY36" s="3"/>
+    </row>
+    <row r="37" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2015</v>
       </c>
@@ -1149,8 +1167,9 @@
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY37" s="3"/>
+    </row>
+    <row r="38" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2016</v>
       </c>
@@ -1171,8 +1190,9 @@
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY38" s="3"/>
+    </row>
+    <row r="39" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -1193,8 +1213,9 @@
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY39" s="3"/>
+    </row>
+    <row r="40" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -1215,8 +1236,9 @@
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY40" s="3"/>
+    </row>
+    <row r="41" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2019</v>
       </c>
@@ -1237,8 +1259,9 @@
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="CY41" s="3"/>
+    </row>
+    <row r="42" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -1256,6 +1279,7 @@
       </c>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
+      <c r="CY42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>